<commit_message>
Versión final al 19-12-16
V 5.0.1 R
</commit_message>
<xml_diff>
--- a/Base_Datos.xlsx
+++ b/Base_Datos.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="76">
   <si>
     <t>TABLAS BEAGLE</t>
   </si>
@@ -141,26 +141,7 @@
     <t>u_vol</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t>Total electrónico 1</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t>er producto</t>
-    </r>
+    <t>Total electrónico 1er producto</t>
   </si>
   <si>
     <t>u_vol_ 2</t>
@@ -172,26 +153,13 @@
     <t>u_vol_ 3</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t>Total electrónico 3</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t>er producto</t>
-    </r>
+    <t>Total electrónico 3er producto</t>
+  </si>
+  <si>
+    <t>idpos</t>
+  </si>
+  <si>
+    <t>Número do posición del corte</t>
   </si>
   <si>
     <t>PRODUCTOS</t>
@@ -212,6 +180,9 @@
     <t>s_diesel</t>
   </si>
   <si>
+    <t>identificador de cara</t>
+  </si>
+  <si>
     <t>RECIBO</t>
   </si>
   <si>
@@ -249,6 +220,36 @@
   </si>
   <si>
     <t>Mensaje al final del recibo</t>
+  </si>
+  <si>
+    <t>idestacion</t>
+  </si>
+  <si>
+    <t>identificador de la EDS</t>
+  </si>
+  <si>
+    <t>RECUPERACION</t>
+  </si>
+  <si>
+    <t>Identificador de cara</t>
+  </si>
+  <si>
+    <t>tot1</t>
+  </si>
+  <si>
+    <t>totales electrónicos manguera 1</t>
+  </si>
+  <si>
+    <t>tot2</t>
+  </si>
+  <si>
+    <t>totales electrónicos manguera 2</t>
+  </si>
+  <si>
+    <t>tot3</t>
+  </si>
+  <si>
+    <t>totales electrónicos manguera 3</t>
   </si>
 </sst>
 </file>
@@ -258,7 +259,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="GENERAL"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -283,14 +284,6 @@
     </font>
     <font>
       <b val="true"/>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <vertAlign val="superscript"/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -359,7 +352,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -390,10 +383,6 @@
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -473,19 +462,19 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E36"/>
+  <dimension ref="A1:E45"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C38" activeCellId="0" sqref="C38"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A34" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C46" activeCellId="0" sqref="C46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.4183673469388"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.1989795918367"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="71.9489795918367"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.9030612244898"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="10.3928571428571"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.2857142857143"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.9285714285714"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="71.1428571428571"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.6326530612245"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="10.2602040816327"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -706,7 +695,7 @@
       <c r="B20" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C20" s="8" t="s">
+      <c r="C20" s="4" t="s">
         <v>39</v>
       </c>
       <c r="D20" s="4"/>
@@ -730,30 +719,30 @@
       <c r="B22" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C22" s="8" t="s">
+      <c r="C22" s="4" t="s">
         <v>43</v>
       </c>
       <c r="D22" s="4"/>
     </row>
-    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="2" t="s">
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="B24" s="2"/>
-      <c r="C24" s="2"/>
-      <c r="D24" s="2"/>
+      <c r="B23" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="D23" s="4"/>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="B25" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="C25" s="4" t="s">
+      <c r="A25" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="D25" s="4"/>
+      <c r="B25" s="2"/>
+      <c r="C25" s="2"/>
+      <c r="D25" s="2"/>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="3" t="s">
@@ -763,121 +752,214 @@
         <v>30</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="D26" s="4"/>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="3" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B27" s="4" t="s">
         <v>30</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="D27" s="4"/>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="3" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B28" s="4" t="s">
         <v>30</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="D28" s="4"/>
     </row>
+    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="B29" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="D29" s="4"/>
+    </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="B30" s="2"/>
-      <c r="C30" s="2"/>
-      <c r="D30" s="2"/>
-    </row>
-    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="B31" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C31" s="4" t="s">
+      <c r="A30" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C30" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="D31" s="4"/>
+      <c r="D30" s="4"/>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="4" t="s">
+      <c r="A32" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="B32" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C32" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="D32" s="4"/>
+      <c r="B32" s="2"/>
+      <c r="C32" s="2"/>
+      <c r="D32" s="2"/>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="B33" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C33" s="4" t="s">
         <v>55</v>
-      </c>
-      <c r="B33" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C33" s="4" t="s">
-        <v>56</v>
       </c>
       <c r="D33" s="4"/>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="B34" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C34" s="4" t="s">
         <v>57</v>
-      </c>
-      <c r="B34" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C34" s="4" t="s">
-        <v>58</v>
       </c>
       <c r="D34" s="4"/>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="B35" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C35" s="4" t="s">
         <v>59</v>
-      </c>
-      <c r="B35" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C35" s="4" t="s">
-        <v>60</v>
       </c>
       <c r="D35" s="4"/>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="B36" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C36" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="B36" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C36" s="4" t="s">
+      <c r="D36" s="4"/>
+    </row>
+    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="D36" s="4"/>
+      <c r="B37" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C37" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="D37" s="4"/>
+    </row>
+    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="B38" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C38" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="D38" s="4"/>
+    </row>
+    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="B39" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C39" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="D39" s="4"/>
+    </row>
+    <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B41" s="2"/>
+      <c r="C41" s="2"/>
+      <c r="D41" s="2"/>
+    </row>
+    <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B42" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C42" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="D42" s="4"/>
+    </row>
+    <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="B43" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C43" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="D43" s="4"/>
+    </row>
+    <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="B44" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C44" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="D44" s="4"/>
+    </row>
+    <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="B45" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C45" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="D45" s="4"/>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="6">
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="A2:D2"/>
     <mergeCell ref="A17:D17"/>
-    <mergeCell ref="A24:D24"/>
-    <mergeCell ref="A30:D30"/>
+    <mergeCell ref="A25:D25"/>
+    <mergeCell ref="A32:D32"/>
+    <mergeCell ref="A41:D41"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -902,7 +984,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="10.3928571428571"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="10.2602040816327"/>
   </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -928,7 +1010,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="10.3928571428571"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="10.2602040816327"/>
   </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>